<commit_message>
Work on champion reward
</commit_message>
<xml_diff>
--- a/Assets/Numbers.xlsx
+++ b/Assets/Numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\unity\Project\LastDevotion\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74272EE-60C4-433A-8D8F-8B8A4DBD0D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA66D888-9FAB-4CA6-8F22-37ACA34B747B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Champion" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
   <si>
     <t>RubyRose</t>
   </si>
@@ -271,9 +271,6 @@
   </si>
   <si>
     <t>50hp-100mp-10mpregen</t>
-  </si>
-  <si>
-    <t>+5 MP, +1.5 MPREGEN</t>
   </si>
   <si>
     <t>Gooze</t>
@@ -305,6 +302,12 @@
   </si>
   <si>
     <t>Eye of the Reaper (active) — Summoning the void’s own sight, she tears open a black hole in the sky. A torrent of dark magic crashes down upon her enemy, dealing 8 × wisdom damage. Each time she is wounded, the Reaper’s eye may awaken again, with a (10 + wisdom × 0.5)% chance to appear above another, untargeted foe.</t>
+  </si>
+  <si>
+    <t>-0.25 MP, +1.5 MPREGEN</t>
+  </si>
+  <si>
+    <t>+15 HP,  +0.1 HPREGEN</t>
   </si>
 </sst>
 </file>
@@ -661,9 +664,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,7 +742,7 @@
         <v>20</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -772,7 +775,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="1">
         <v>50</v>
@@ -1066,7 +1069,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="1">
         <v>34</v>
@@ -1399,7 +1402,7 @@
         <v>36</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15" s="1">
         <v>34</v>
@@ -1771,7 +1774,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" s="1">
         <v>38</v>
@@ -2006,7 +2009,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2151,10 +2154,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117DB8B5-5D2C-4497-B733-052439D374C4}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="B12:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2181,6 +2184,9 @@
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="B3">
+        <v>-0.6</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
@@ -2190,7 +2196,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
         <v>63</v>
@@ -2221,7 +2227,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
         <v>65</v>
@@ -2279,6 +2285,9 @@
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="B10">
+        <v>0.03</v>
+      </c>
       <c r="E10" t="s">
         <v>68</v>
       </c>
@@ -2324,6 +2333,11 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>3.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish champion reward & Add some dev commands
</commit_message>
<xml_diff>
--- a/Assets/Numbers.xlsx
+++ b/Assets/Numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\unity\Project\LastDevotion\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EB00AF-91CC-4BED-8519-AB8109D9A8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96569725-EC3E-4771-A716-6AA5FBC4B7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
   <si>
     <t>RubyRose</t>
   </si>
@@ -308,6 +308,10 @@
   </si>
   <si>
     <t>+15 HP,  +0.1 HPREGEN</t>
+  </si>
+  <si>
+    <t>Goo Rush (active)
+Slows all nearby enemies by 50% for 4.5 seconds, then leaps to the nearest ally, granting them +0.25 Attack Speed for 2 seconds.</t>
   </si>
 </sst>
 </file>
@@ -665,8 +669,8 @@
   <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:S4"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2007,9 +2011,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>74</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish Gooze & Work on Elite Mukai
</commit_message>
<xml_diff>
--- a/Assets/Numbers.xlsx
+++ b/Assets/Numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\unity\Project\LastDevotion\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96569725-EC3E-4771-A716-6AA5FBC4B7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DD266C-8F37-48AD-83F7-79C2F09609C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -311,7 +311,7 @@
   </si>
   <si>
     <t>Goo Rush (active)
-Slows all nearby enemies by 50% for 4.5 seconds, then leaps to the nearest ally, granting them +0.25 Attack Speed for 2 seconds.</t>
+Slows all nearby enemies by (0.5 + Might × 0.01) for 4.5 seconds, then leaps to the nearest ally, granting them (0.3 + Reflex × 0.01) Attack Speed for 3.5 seconds. If no allies are present, the effect is applied to himself instead.</t>
   </si>
 </sst>
 </file>
@@ -2011,12 +2011,66 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>82</v>
+      </c>
+      <c r="C25" s="1">
+        <v>50</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>55</v>
+      </c>
+      <c r="F25" s="1">
+        <v>10</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K25" s="1">
+        <v>1</v>
+      </c>
+      <c r="L25" s="1">
+        <v>2</v>
+      </c>
+      <c r="M25" s="1">
+        <v>1</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0</v>
+      </c>
+      <c r="O25" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="P25" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>1</v>
+      </c>
+      <c r="R25" s="1">
+        <v>0</v>
+      </c>
+      <c r="S25" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="T25" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done Mukai [Active: TremorBreak & Passive: FeralAwakening]
</commit_message>
<xml_diff>
--- a/Assets/Numbers.xlsx
+++ b/Assets/Numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\unity\Project\LastDevotion\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DD266C-8F37-48AD-83F7-79C2F09609C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAB5F59-9E4F-435E-95CA-4B6E6D72E95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="84">
   <si>
     <t>RubyRose</t>
   </si>
@@ -312,6 +312,9 @@
   <si>
     <t>Goo Rush (active)
 Slows all nearby enemies by (0.5 + Might × 0.01) for 4.5 seconds, then leaps to the nearest ally, granting them (0.3 + Reflex × 0.01) Attack Speed for 3.5 seconds. If no allies are present, the effect is applied to himself instead.</t>
+  </si>
+  <si>
+    <t>Mukai</t>
   </si>
 </sst>
 </file>
@@ -666,11 +669,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2072,6 +2075,68 @@
       <c r="T25" s="1">
         <v>1</v>
       </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="1">
+        <v>100</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>50</v>
+      </c>
+      <c r="F26" s="1">
+        <v>10</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+      <c r="K26" s="1">
+        <v>1</v>
+      </c>
+      <c r="L26" s="1">
+        <v>2</v>
+      </c>
+      <c r="M26" s="1">
+        <v>1</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0</v>
+      </c>
+      <c r="O26" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="P26" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>1</v>
+      </c>
+      <c r="R26" s="1">
+        <v>0</v>
+      </c>
+      <c r="S26" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="T26" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prepare adding more items
</commit_message>
<xml_diff>
--- a/Assets/Numbers.xlsx
+++ b/Assets/Numbers.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\unity\Project\LastDevotion\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5545742F-3AC9-46FF-BE28-C3A6646B53F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924C433F-4A66-4F63-AF92-09B821882059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Champion" sheetId="1" r:id="rId1"/>
     <sheet name="Stat" sheetId="2" r:id="rId2"/>
     <sheet name="Experiment" sheetId="3" r:id="rId3"/>
+    <sheet name="Item" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,8 +38,480 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="46">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="3"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="4"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="5"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="6"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="7"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="8"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="9"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="10"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="11"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="12"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="13"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="14"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="15"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="16"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="17"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="18"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="19"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="20"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="21"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="22"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="23"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="24"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="25"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="26"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="27"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="28"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="29"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="30"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="31"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="32"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="33"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="34"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="35"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="36"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="37"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="38"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="39"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="40"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="41"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="42"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="43"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="44"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="45"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="46">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
+    <bk>
+      <rc t="1" v="3"/>
+    </bk>
+    <bk>
+      <rc t="1" v="4"/>
+    </bk>
+    <bk>
+      <rc t="1" v="5"/>
+    </bk>
+    <bk>
+      <rc t="1" v="6"/>
+    </bk>
+    <bk>
+      <rc t="1" v="7"/>
+    </bk>
+    <bk>
+      <rc t="1" v="8"/>
+    </bk>
+    <bk>
+      <rc t="1" v="9"/>
+    </bk>
+    <bk>
+      <rc t="1" v="10"/>
+    </bk>
+    <bk>
+      <rc t="1" v="11"/>
+    </bk>
+    <bk>
+      <rc t="1" v="12"/>
+    </bk>
+    <bk>
+      <rc t="1" v="13"/>
+    </bk>
+    <bk>
+      <rc t="1" v="14"/>
+    </bk>
+    <bk>
+      <rc t="1" v="15"/>
+    </bk>
+    <bk>
+      <rc t="1" v="16"/>
+    </bk>
+    <bk>
+      <rc t="1" v="17"/>
+    </bk>
+    <bk>
+      <rc t="1" v="18"/>
+    </bk>
+    <bk>
+      <rc t="1" v="19"/>
+    </bk>
+    <bk>
+      <rc t="1" v="20"/>
+    </bk>
+    <bk>
+      <rc t="1" v="21"/>
+    </bk>
+    <bk>
+      <rc t="1" v="22"/>
+    </bk>
+    <bk>
+      <rc t="1" v="23"/>
+    </bk>
+    <bk>
+      <rc t="1" v="24"/>
+    </bk>
+    <bk>
+      <rc t="1" v="25"/>
+    </bk>
+    <bk>
+      <rc t="1" v="26"/>
+    </bk>
+    <bk>
+      <rc t="1" v="27"/>
+    </bk>
+    <bk>
+      <rc t="1" v="28"/>
+    </bk>
+    <bk>
+      <rc t="1" v="29"/>
+    </bk>
+    <bk>
+      <rc t="1" v="30"/>
+    </bk>
+    <bk>
+      <rc t="1" v="31"/>
+    </bk>
+    <bk>
+      <rc t="1" v="32"/>
+    </bk>
+    <bk>
+      <rc t="1" v="33"/>
+    </bk>
+    <bk>
+      <rc t="1" v="34"/>
+    </bk>
+    <bk>
+      <rc t="1" v="35"/>
+    </bk>
+    <bk>
+      <rc t="1" v="36"/>
+    </bk>
+    <bk>
+      <rc t="1" v="37"/>
+    </bk>
+    <bk>
+      <rc t="1" v="38"/>
+    </bk>
+    <bk>
+      <rc t="1" v="39"/>
+    </bk>
+    <bk>
+      <rc t="1" v="40"/>
+    </bk>
+    <bk>
+      <rc t="1" v="41"/>
+    </bk>
+    <bk>
+      <rc t="1" v="42"/>
+    </bk>
+    <bk>
+      <rc t="1" v="43"/>
+    </bk>
+    <bk>
+      <rc t="1" v="44"/>
+    </bk>
+    <bk>
+      <rc t="1" v="45"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="150">
   <si>
     <t>RubyRose</t>
   </si>
@@ -321,6 +794,198 @@
   </si>
   <si>
     <t>Feral Awakening: Dropping under 50% HP triggers a 2-second Focus Stance, rooting you in place as primal energy gathers. Afterward, you shift into a melee form—trading range for ferocity and gaining (2 + 0.01 × Might) attack speed and (1000 + 10 × Might) bonus HP.</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>BF</t>
+  </si>
+  <si>
+    <t>RB</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>NLR</t>
+  </si>
+  <si>
+    <t>TOTG</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>EON</t>
+  </si>
+  <si>
+    <t>BT</t>
+  </si>
+  <si>
+    <t>HG</t>
+  </si>
+  <si>
+    <t>SOS</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>SFE</t>
+  </si>
+  <si>
+    <t>ELE</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>KF</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>VS</t>
+  </si>
+  <si>
+    <t>NT</t>
+  </si>
+  <si>
+    <t>LW</t>
+  </si>
+  <si>
+    <t>SCE</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>BV</t>
+  </si>
+  <si>
+    <t>CG</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SF </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC </t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>WE</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>AH</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>QS</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>JE</t>
+  </si>
+  <si>
+    <t>RD</t>
+  </si>
+  <si>
+    <t>AAS</t>
+  </si>
+  <si>
+    <t>MRL</t>
+  </si>
+  <si>
+    <t>JG</t>
+  </si>
+  <si>
+    <t>SGE</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>SV</t>
+  </si>
+  <si>
+    <t>HOJ</t>
+  </si>
+  <si>
+    <t>BAE</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>CGE</t>
+  </si>
+  <si>
+    <t>HWE</t>
+  </si>
+  <si>
+    <t>TG</t>
+  </si>
+  <si>
+    <t>LE</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>TS</t>
+  </si>
+  <si>
+    <t>Is Index Unique</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -370,7 +1035,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -394,9 +1059,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,6 +1074,295 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="46">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>3</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>4</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>5</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>6</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>7</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>8</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>9</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>10</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>11</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>12</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>13</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>14</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>15</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>16</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>17</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>18</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>19</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>20</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>21</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>22</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>23</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>24</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>25</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>26</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>27</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>28</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>29</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>30</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>31</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>32</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>33</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>34</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>35</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>36</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>37</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>38</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>39</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>40</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>41</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>42</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>43</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>44</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>45</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
+  <rel r:id="rId4"/>
+  <rel r:id="rId5"/>
+  <rel r:id="rId6"/>
+  <rel r:id="rId7"/>
+  <rel r:id="rId8"/>
+  <rel r:id="rId9"/>
+  <rel r:id="rId10"/>
+  <rel r:id="rId11"/>
+  <rel r:id="rId12"/>
+  <rel r:id="rId13"/>
+  <rel r:id="rId14"/>
+  <rel r:id="rId15"/>
+  <rel r:id="rId16"/>
+  <rel r:id="rId17"/>
+  <rel r:id="rId18"/>
+  <rel r:id="rId19"/>
+  <rel r:id="rId20"/>
+  <rel r:id="rId21"/>
+  <rel r:id="rId22"/>
+  <rel r:id="rId23"/>
+  <rel r:id="rId24"/>
+  <rel r:id="rId25"/>
+  <rel r:id="rId26"/>
+  <rel r:id="rId27"/>
+  <rel r:id="rId28"/>
+  <rel r:id="rId29"/>
+  <rel r:id="rId30"/>
+  <rel r:id="rId31"/>
+  <rel r:id="rId32"/>
+  <rel r:id="rId33"/>
+  <rel r:id="rId34"/>
+  <rel r:id="rId35"/>
+  <rel r:id="rId36"/>
+  <rel r:id="rId37"/>
+  <rel r:id="rId38"/>
+  <rel r:id="rId39"/>
+  <rel r:id="rId40"/>
+  <rel r:id="rId41"/>
+  <rel r:id="rId42"/>
+  <rel r:id="rId43"/>
+  <rel r:id="rId44"/>
+  <rel r:id="rId45"/>
+  <rel r:id="rId46"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -680,7 +1631,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
     </sheetView>
@@ -2149,7 +3100,7 @@
     </row>
     <row r="27" spans="1:20" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="1" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2164,7 +3115,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B18"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2298,7 +3249,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2484,4 +3435,914 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF4F598-B7D1-4751-B491-BD0874E7F79E}">
+  <dimension ref="A1:E66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B2">
+        <v>2866</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(COUNTIF($B$2:$B$1000, B2)&gt;1, "Duplicate", "Unique")</f>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B3">
+        <v>2869</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E66" si="0">IF(COUNTIF($B$2:$B$1000, B3)&gt;1, "Duplicate", "Unique")</f>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B4">
+        <v>2478</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B5">
+        <v>2313</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B6">
+        <v>2835</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="e" vm="6">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B7">
+        <v>1633</v>
+      </c>
+      <c r="C7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="e" vm="7">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B8">
+        <v>2334</v>
+      </c>
+      <c r="C8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B9">
+        <v>2339</v>
+      </c>
+      <c r="C9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="e" vm="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B10">
+        <v>821</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="e" vm="10">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B11">
+        <v>823</v>
+      </c>
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="e" vm="11">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B12">
+        <v>2137</v>
+      </c>
+      <c r="C12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B13">
+        <v>3631</v>
+      </c>
+      <c r="C13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="e" vm="13">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B14">
+        <v>2197</v>
+      </c>
+      <c r="C14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="e" vm="14">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B15">
+        <v>2214</v>
+      </c>
+      <c r="C15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="e" vm="15">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B16">
+        <v>2218</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="e" vm="16">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B17">
+        <v>2114</v>
+      </c>
+      <c r="C17" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="e" vm="17">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B18">
+        <v>2220</v>
+      </c>
+      <c r="C18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="e" vm="18">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B19">
+        <v>2234</v>
+      </c>
+      <c r="C19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="e" vm="19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B22">
+        <v>2238</v>
+      </c>
+      <c r="C22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="e" vm="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B23">
+        <v>2243</v>
+      </c>
+      <c r="C23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="e" vm="21">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B24">
+        <v>2264</v>
+      </c>
+      <c r="C24" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="e" vm="22">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B25">
+        <v>2265</v>
+      </c>
+      <c r="C25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="e" vm="23">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B26">
+        <v>2267</v>
+      </c>
+      <c r="C26" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" t="e" vm="24">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B27">
+        <v>2771</v>
+      </c>
+      <c r="C27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="e" vm="25">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B28">
+        <v>2772</v>
+      </c>
+      <c r="C28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>113</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>114</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="e" vm="26">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B31">
+        <v>2308</v>
+      </c>
+      <c r="C31" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="e" vm="27">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B32">
+        <v>2312</v>
+      </c>
+      <c r="C32" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="e" vm="28">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B33">
+        <v>2305</v>
+      </c>
+      <c r="C33" t="s">
+        <v>116</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="e" vm="29">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B34">
+        <v>2309</v>
+      </c>
+      <c r="C34" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" t="e" vm="30">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B35">
+        <v>2287</v>
+      </c>
+      <c r="C35" t="s">
+        <v>119</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="e" vm="31">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B36">
+        <v>2317</v>
+      </c>
+      <c r="C36" t="s">
+        <v>120</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>121</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="e" vm="32">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B39">
+        <v>2337</v>
+      </c>
+      <c r="C39" t="s">
+        <v>123</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="e" vm="33">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B40">
+        <v>2347</v>
+      </c>
+      <c r="C40" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" t="e" vm="34">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B41">
+        <v>2346</v>
+      </c>
+      <c r="C41" t="s">
+        <v>125</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="e" vm="35">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B42">
+        <v>2325</v>
+      </c>
+      <c r="C42" t="s">
+        <v>126</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="e" vm="36">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B43">
+        <v>2330</v>
+      </c>
+      <c r="C43" t="s">
+        <v>127</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>128</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>129</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" t="e" vm="37">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B46">
+        <v>2358</v>
+      </c>
+      <c r="C46" t="s">
+        <v>130</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="e" vm="38">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B47">
+        <v>2497</v>
+      </c>
+      <c r="C47" t="s">
+        <v>131</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" t="e" vm="39">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B48">
+        <v>2524</v>
+      </c>
+      <c r="C48" t="s">
+        <v>132</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" t="e" vm="40">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B49">
+        <v>2621</v>
+      </c>
+      <c r="C49" t="s">
+        <v>133</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>134</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>128</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" t="e" vm="41">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B52">
+        <v>2618</v>
+      </c>
+      <c r="C52" t="s">
+        <v>135</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" t="e" vm="42">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B53">
+        <v>2620</v>
+      </c>
+      <c r="C53" t="s">
+        <v>136</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" t="e" vm="43">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B54">
+        <v>2630</v>
+      </c>
+      <c r="C54" t="s">
+        <v>137</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>138</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>139</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" t="e" vm="44">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B57">
+        <v>2634</v>
+      </c>
+      <c r="C57" t="s">
+        <v>140</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" t="e" vm="45">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B58">
+        <v>2848</v>
+      </c>
+      <c r="C58" t="s">
+        <v>118</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>141</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>142</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" t="e" vm="46">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B61">
+        <v>2888</v>
+      </c>
+      <c r="C61" t="s">
+        <v>143</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>144</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
+        <v>145</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <v>4491</v>
+      </c>
+      <c r="C64" t="s">
+        <v>146</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>3184</v>
+      </c>
+      <c r="C65" t="s">
+        <v>146</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>3182</v>
+      </c>
+      <c r="C66" t="s">
+        <v>147</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="0"/>
+        <v>Unique</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Work on item reward
</commit_message>
<xml_diff>
--- a/Assets/Numbers.xlsx
+++ b/Assets/Numbers.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\unity\Project\LastDevotion\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924C433F-4A66-4F63-AF92-09B821882059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A462FC-A684-4146-A428-D78007221B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Champion" sheetId="1" r:id="rId1"/>
-    <sheet name="Stat" sheetId="2" r:id="rId2"/>
-    <sheet name="Experiment" sheetId="3" r:id="rId3"/>
-    <sheet name="Item" sheetId="4" r:id="rId4"/>
+    <sheet name="CHAMPION" sheetId="1" r:id="rId1"/>
+    <sheet name="STAT" sheetId="2" r:id="rId2"/>
+    <sheet name="EXPERIMENT" sheetId="3" r:id="rId3"/>
+    <sheet name="ITEM" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -511,7 +511,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="169">
   <si>
     <t>RubyRose</t>
   </si>
@@ -689,13 +689,7 @@
 The impact then solidifies into jagged icicles beneath the enemy’s feet, impaling them and dealing 1 × atk damage per second.</t>
   </si>
   <si>
-    <t>+22 HP,  +0.1 HPREGEN</t>
-  </si>
-  <si>
     <t>+0.17 ARMOR, +0.01 ASPD</t>
-  </si>
-  <si>
-    <t>+12 MP, +0.05 MPREGEN</t>
   </si>
   <si>
     <t>Might</t>
@@ -802,57 +796,18 @@
     <t>Name</t>
   </si>
   <si>
-    <t>BF</t>
-  </si>
-  <si>
     <t>RB</t>
   </si>
   <si>
-    <t>CV</t>
-  </si>
-  <si>
-    <t>NC</t>
-  </si>
-  <si>
-    <t>NLR</t>
-  </si>
-  <si>
-    <t>TOTG</t>
-  </si>
-  <si>
-    <t>GB</t>
-  </si>
-  <si>
-    <t>SG</t>
-  </si>
-  <si>
     <t>ST</t>
   </si>
   <si>
     <t>FP</t>
   </si>
   <si>
-    <t>DB</t>
-  </si>
-  <si>
     <t>GS</t>
   </si>
   <si>
-    <t>EON</t>
-  </si>
-  <si>
-    <t>BT</t>
-  </si>
-  <si>
-    <t>HG</t>
-  </si>
-  <si>
-    <t>SOS</t>
-  </si>
-  <si>
-    <t>IE</t>
-  </si>
-  <si>
     <t>SFE</t>
   </si>
   <si>
@@ -986,6 +941,123 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>+2 ATK</t>
+  </si>
+  <si>
+    <t>+0.1 ASPD</t>
+  </si>
+  <si>
+    <t>+0.8 ARMOR</t>
+  </si>
+  <si>
+    <t>-1 MP</t>
+  </si>
+  <si>
+    <t>+0.06 OMNIVAMP</t>
+  </si>
+  <si>
+    <t>+2.8 MPREGEN</t>
+  </si>
+  <si>
+    <t>+30 HP</t>
+  </si>
+  <si>
+    <t>+10 ATK</t>
+  </si>
+  <si>
+    <t>+4.5 ATK
++0.15 ASPD
+Deal 15% more damage against enemies with higher HP than you.</t>
+  </si>
+  <si>
+    <t>+3 ARMOR
++5 ATK
+At 50% HP, briefly gain 100xHP.</t>
+  </si>
+  <si>
+    <t>55hp, 25curhp, 12*2.5 armor</t>
+  </si>
+  <si>
+    <t>-5 MP
++5.5 ATK
+At 40% HP, 50% CURHP is converted to ARMOR for 5s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+4.25 ATK
++0.2 OMNIVAMP
+Heal lowest CURHP ally for 25% of damage dealt.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100hp, 60curhp, </t>
+  </si>
+  <si>
+    <t>+2.5 ATK
++3 MPREGEN
+Attack grant 4 MP.</t>
+  </si>
+  <si>
+    <t>+4.75 ATK
++100 HP
+At 60% HP, gain 100% fake HP that decay over 4s.</t>
+  </si>
+  <si>
+    <t>+0.15 CRIT</t>
+  </si>
+  <si>
+    <t>+4 ATK
++0.3 CRIT
+Abilities can critical strike.</t>
+  </si>
+  <si>
+    <t>Ironshard</t>
+  </si>
+  <si>
+    <t>Quickbrand</t>
+  </si>
+  <si>
+    <t>Rusted Chainmail</t>
+  </si>
+  <si>
+    <t>Seepcloak</t>
+  </si>
+  <si>
+    <t>Leechwood Rod</t>
+  </si>
+  <si>
+    <t>Oakspan Gloves</t>
+  </si>
+  <si>
+    <t>Embervein</t>
+  </si>
+  <si>
+    <t>Piercehand</t>
+  </si>
+  <si>
+    <t>Astraquill Sabre</t>
+  </si>
+  <si>
+    <t>Viridian Bolt</t>
+  </si>
+  <si>
+    <t>Frostlink</t>
+  </si>
+  <si>
+    <t>Battlemask</t>
+  </si>
+  <si>
+    <t>Nightbrew Vessel</t>
+  </si>
+  <si>
+    <t>Fleshgrip</t>
+  </si>
+  <si>
+    <t>Sunmane Bastion</t>
+  </si>
+  <si>
+    <t>Grimcircuit</t>
   </si>
 </sst>
 </file>
@@ -1035,7 +1107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1058,6 +1130,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1709,7 +1784,7 @@
         <v>20</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -1742,7 +1817,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" s="1">
         <v>50</v>
@@ -2036,7 +2111,7 @@
         <v>30</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C9" s="1">
         <v>34</v>
@@ -2369,7 +2444,7 @@
         <v>36</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C15" s="1">
         <v>34</v>
@@ -2741,7 +2816,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C21" s="1">
         <v>38</v>
@@ -2976,10 +3051,10 @@
     </row>
     <row r="25" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C25" s="1">
         <v>50</v>
@@ -3038,10 +3113,10 @@
     </row>
     <row r="26" spans="1:20" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C26" s="1">
         <v>100</v>
@@ -3101,7 +3176,7 @@
     <row r="27" spans="1:20" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3115,7 +3190,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3128,7 +3203,7 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="7"/>
       <c r="B1" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3159,16 +3234,16 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>55</v>
+      <c r="B6" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>56</v>
+      <c r="B7" s="6" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3176,7 +3251,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -3246,10 +3321,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117DB8B5-5D2C-4497-B733-052439D374C4}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3261,7 +3336,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -3282,47 +3357,47 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F6">
         <v>125</v>
@@ -3342,7 +3417,7 @@
         <v>0.02</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F7">
         <v>105</v>
@@ -3370,7 +3445,7 @@
         <v>0.05</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -3381,7 +3456,7 @@
         <v>0.03</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F10">
         <v>12.5</v>
@@ -3395,7 +3470,7 @@
         <v>0.4</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F11">
         <v>17</v>
@@ -3411,7 +3486,7 @@
         <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -3419,17 +3494,27 @@
         <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17">
         <v>3.8</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3441,29 +3526,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF4F598-B7D1-4751-B491-BD0874E7F79E}">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" customWidth="1"/>
     <col min="5" max="5" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -3474,7 +3560,10 @@
         <v>2866</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>153</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="E2" t="str">
         <f>IF(COUNTIF($B$2:$B$1000, B2)&gt;1, "Duplicate", "Unique")</f>
@@ -3489,7 +3578,10 @@
         <v>2869</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>154</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E66" si="0">IF(COUNTIF($B$2:$B$1000, B3)&gt;1, "Duplicate", "Unique")</f>
@@ -3504,7 +3596,10 @@
         <v>2478</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>155</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -3519,7 +3614,10 @@
         <v>2313</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>156</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -3534,7 +3632,10 @@
         <v>2835</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>157</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -3549,7 +3650,10 @@
         <v>1633</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>159</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -3564,7 +3668,10 @@
         <v>2334</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>158</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -3579,7 +3686,10 @@
         <v>2339</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>160</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -3594,7 +3704,7 @@
         <v>821</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -3609,7 +3719,7 @@
         <v>823</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -3624,29 +3734,35 @@
         <v>2137</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
+        <v>161</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
         <v>Unique</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
       <c r="B13">
-        <v>3631</v>
+        <v>2143</v>
       </c>
       <c r="C13" t="s">
-        <v>99</v>
+        <v>162</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>143</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
         <v>Unique</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
@@ -3654,14 +3770,17 @@
         <v>2197</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>163</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
         <v>Unique</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
@@ -3669,14 +3788,17 @@
         <v>2214</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>164</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
         <v>Unique</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
@@ -3684,7 +3806,10 @@
         <v>2218</v>
       </c>
       <c r="C16" t="s">
-        <v>102</v>
+        <v>165</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>147</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
@@ -3699,14 +3824,17 @@
         <v>2114</v>
       </c>
       <c r="C17" t="s">
-        <v>103</v>
+        <v>166</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>149</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
         <v>Unique</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="e" vm="17">
         <v>#VALUE!</v>
       </c>
@@ -3714,14 +3842,17 @@
         <v>2220</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>167</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>150</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
         <v>Unique</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
@@ -3729,7 +3860,10 @@
         <v>2234</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>168</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>152</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
@@ -3738,13 +3872,13 @@
     </row>
     <row r="20" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
@@ -3753,7 +3887,7 @@
     </row>
     <row r="21" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
@@ -3768,7 +3902,7 @@
         <v>2238</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
@@ -3783,7 +3917,7 @@
         <v>2243</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
@@ -3798,7 +3932,7 @@
         <v>2264</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
@@ -3813,7 +3947,7 @@
         <v>2265</v>
       </c>
       <c r="C25" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
@@ -3828,7 +3962,7 @@
         <v>2267</v>
       </c>
       <c r="C26" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
@@ -3843,7 +3977,7 @@
         <v>2771</v>
       </c>
       <c r="C27" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
@@ -3858,7 +3992,7 @@
         <v>2772</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
@@ -3867,7 +4001,7 @@
     </row>
     <row r="29" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
@@ -3876,7 +4010,7 @@
     </row>
     <row r="30" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
@@ -3891,7 +4025,7 @@
         <v>2308</v>
       </c>
       <c r="C31" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
@@ -3906,7 +4040,7 @@
         <v>2312</v>
       </c>
       <c r="C32" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
@@ -3921,7 +4055,7 @@
         <v>2305</v>
       </c>
       <c r="C33" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
@@ -3936,7 +4070,7 @@
         <v>2309</v>
       </c>
       <c r="C34" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
@@ -3951,7 +4085,7 @@
         <v>2287</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
@@ -3966,7 +4100,7 @@
         <v>2317</v>
       </c>
       <c r="C36" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
@@ -3975,7 +4109,7 @@
     </row>
     <row r="37" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
@@ -3984,7 +4118,7 @@
     </row>
     <row r="38" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
@@ -3999,7 +4133,7 @@
         <v>2337</v>
       </c>
       <c r="C39" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
@@ -4014,7 +4148,7 @@
         <v>2347</v>
       </c>
       <c r="C40" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
@@ -4029,7 +4163,7 @@
         <v>2346</v>
       </c>
       <c r="C41" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
@@ -4044,7 +4178,7 @@
         <v>2325</v>
       </c>
       <c r="C42" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
@@ -4059,7 +4193,7 @@
         <v>2330</v>
       </c>
       <c r="C43" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
@@ -4068,7 +4202,7 @@
     </row>
     <row r="44" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
@@ -4077,7 +4211,7 @@
     </row>
     <row r="45" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
@@ -4092,7 +4226,7 @@
         <v>2358</v>
       </c>
       <c r="C46" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
@@ -4107,7 +4241,7 @@
         <v>2497</v>
       </c>
       <c r="C47" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
@@ -4122,7 +4256,7 @@
         <v>2524</v>
       </c>
       <c r="C48" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
@@ -4137,7 +4271,7 @@
         <v>2621</v>
       </c>
       <c r="C49" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
@@ -4146,7 +4280,7 @@
     </row>
     <row r="50" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
@@ -4155,7 +4289,7 @@
     </row>
     <row r="51" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
@@ -4170,7 +4304,7 @@
         <v>2618</v>
       </c>
       <c r="C52" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="0"/>
@@ -4185,7 +4319,7 @@
         <v>2620</v>
       </c>
       <c r="C53" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="E53" t="str">
         <f t="shared" si="0"/>
@@ -4200,7 +4334,7 @@
         <v>2630</v>
       </c>
       <c r="C54" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" si="0"/>
@@ -4209,7 +4343,7 @@
     </row>
     <row r="55" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
@@ -4218,7 +4352,7 @@
     </row>
     <row r="56" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
@@ -4233,7 +4367,7 @@
         <v>2634</v>
       </c>
       <c r="C57" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E57" t="str">
         <f t="shared" si="0"/>
@@ -4248,7 +4382,7 @@
         <v>2848</v>
       </c>
       <c r="C58" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" si="0"/>
@@ -4257,7 +4391,7 @@
     </row>
     <row r="59" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="E59" t="str">
         <f t="shared" si="0"/>
@@ -4266,7 +4400,7 @@
     </row>
     <row r="60" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" si="0"/>
@@ -4281,7 +4415,7 @@
         <v>2888</v>
       </c>
       <c r="C61" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="0"/>
@@ -4290,7 +4424,7 @@
     </row>
     <row r="62" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="0"/>
@@ -4299,7 +4433,7 @@
     </row>
     <row r="63" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="E63" t="str">
         <f t="shared" si="0"/>
@@ -4311,7 +4445,7 @@
         <v>4491</v>
       </c>
       <c r="C64" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="E64" t="str">
         <f t="shared" si="0"/>
@@ -4323,7 +4457,7 @@
         <v>3184</v>
       </c>
       <c r="C65" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="E65" t="str">
         <f t="shared" si="0"/>
@@ -4335,7 +4469,7 @@
         <v>3182</v>
       </c>
       <c r="C66" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="E66" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Work on item reward (2)
</commit_message>
<xml_diff>
--- a/Assets/Numbers.xlsx
+++ b/Assets/Numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\unity\Project\LastDevotion\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A462FC-A684-4146-A428-D78007221B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FF5551-A32A-4363-AC98-99A0E563B9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="72" yWindow="1584" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAMPION" sheetId="1" r:id="rId1"/>
@@ -3526,8 +3526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF4F598-B7D1-4751-B491-BD0874E7F79E}">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Small tweak on reward and enemy
</commit_message>
<xml_diff>
--- a/Assets/Numbers.xlsx
+++ b/Assets/Numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\unity\Project\LastDevotion\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FF5551-A32A-4363-AC98-99A0E563B9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1349893-A84D-4E0B-B4D9-BA37E841C5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72" yWindow="1584" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAMPION" sheetId="1" r:id="rId1"/>
@@ -3526,8 +3526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF4F598-B7D1-4751-B491-BD0874E7F79E}">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Work on shop (3) & improve map
</commit_message>
<xml_diff>
--- a/Assets/Numbers.xlsx
+++ b/Assets/Numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\unity\Project\LastDevotion\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1349893-A84D-4E0B-B4D9-BA37E841C5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6467842-AE58-4A2A-B017-FF18BCB4F86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAMPION" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="171">
   <si>
     <t>RubyRose</t>
   </si>
@@ -1058,6 +1058,12 @@
   </si>
   <si>
     <t>Grimcircuit</t>
+  </si>
+  <si>
+    <t>PRICE</t>
+  </si>
+  <si>
+    <t>GOLD DROP</t>
   </si>
 </sst>
 </file>
@@ -1704,11 +1710,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T27"/>
+  <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1723,9 +1731,10 @@
     <col min="17" max="17" width="10.109375" customWidth="1"/>
     <col min="18" max="18" width="12.77734375" customWidth="1"/>
     <col min="19" max="19" width="12.44140625" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1786,8 +1795,14 @@
       <c r="T1" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1812,7 +1827,7 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:20" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1873,8 +1888,14 @@
       <c r="T3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U3" s="1">
+        <v>60</v>
+      </c>
+      <c r="V3" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1933,10 +1954,16 @@
         <v>1.25</v>
       </c>
       <c r="T4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="U4" s="1">
+        <v>65</v>
+      </c>
+      <c r="V4" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1997,8 +2024,14 @@
       <c r="T5" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U5" s="1">
+        <v>200</v>
+      </c>
+      <c r="V5" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>24</v>
@@ -2021,7 +2054,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:20" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -2082,8 +2115,14 @@
       <c r="T7" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="U7" s="1">
+        <v>125</v>
+      </c>
+      <c r="V7" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
         <v>27</v>
@@ -2106,7 +2145,7 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:20" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2167,8 +2206,14 @@
       <c r="T9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="U9" s="1">
+        <v>70</v>
+      </c>
+      <c r="V9" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -2229,8 +2274,14 @@
       <c r="T10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U10" s="1">
+        <v>55</v>
+      </c>
+      <c r="V10" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -2291,8 +2342,14 @@
       <c r="T11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="U11" s="1">
+        <v>50</v>
+      </c>
+      <c r="V11" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -2353,8 +2410,14 @@
       <c r="T12" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="U12" s="1">
+        <v>100</v>
+      </c>
+      <c r="V12" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="5" t="s">
         <v>53</v>
@@ -2377,7 +2440,7 @@
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
     </row>
-    <row r="14" spans="1:20" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -2438,8 +2501,14 @@
       <c r="T14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" ht="232.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U14" s="1">
+        <v>58</v>
+      </c>
+      <c r="V14" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="232.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -2500,8 +2569,14 @@
       <c r="T15" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="U15" s="1">
+        <v>120</v>
+      </c>
+      <c r="V15" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
@@ -2562,8 +2637,14 @@
       <c r="T16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="U16" s="1">
+        <v>60</v>
+      </c>
+      <c r="V16" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
@@ -2624,8 +2705,14 @@
       <c r="T17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="U17" s="1">
+        <v>62</v>
+      </c>
+      <c r="V17" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
@@ -2686,8 +2773,14 @@
       <c r="T18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="U18" s="1">
+        <v>52</v>
+      </c>
+      <c r="V18" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
@@ -2748,8 +2841,14 @@
       <c r="T19" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U19" s="1">
+        <v>115</v>
+      </c>
+      <c r="V19" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
@@ -2810,8 +2909,14 @@
       <c r="T20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="U20" s="1">
+        <v>54</v>
+      </c>
+      <c r="V20" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -2872,8 +2977,14 @@
       <c r="T21" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U21" s="1">
+        <v>215</v>
+      </c>
+      <c r="V21" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>46</v>
       </c>
@@ -2930,7 +3041,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
@@ -2987,7 +3098,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>49</v>
       </c>
@@ -3048,8 +3159,14 @@
       <c r="T24" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="U24" s="1">
+        <v>64</v>
+      </c>
+      <c r="V24" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
@@ -3110,8 +3227,14 @@
       <c r="T25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U25" s="1">
+        <v>67</v>
+      </c>
+      <c r="V25" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>81</v>
       </c>
@@ -3170,10 +3293,16 @@
         <v>1.25</v>
       </c>
       <c r="T26" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="U26" s="1">
+        <v>350</v>
+      </c>
+      <c r="V26" s="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>83</v>
@@ -3526,8 +3655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF4F598-B7D1-4751-B491-BD0874E7F79E}">
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:E14"/>
+    <sheetView topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Work on shop (4)
</commit_message>
<xml_diff>
--- a/Assets/Numbers.xlsx
+++ b/Assets/Numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\unity\Project\LastDevotion\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6467842-AE58-4A2A-B017-FF18BCB4F86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99A1D89-BB44-4F34-941F-1A98904242A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAMPION" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="172">
   <si>
     <t>RubyRose</t>
   </si>
@@ -1064,6 +1064,9 @@
   </si>
   <si>
     <t>GOLD DROP</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -1712,11 +1715,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W24" sqref="W24"/>
+      <selection pane="bottomRight" activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1827,21 +1830,21 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:22" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="F3" s="1">
         <v>10</v>
@@ -1859,7 +1862,7 @@
         <v>0.8</v>
       </c>
       <c r="K3" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L3" s="1">
         <v>2</v>
@@ -1886,98 +1889,53 @@
         <v>1.25</v>
       </c>
       <c r="T3" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U3" s="1">
-        <v>60</v>
+        <v>200</v>
       </c>
       <c r="V3" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
       <c r="B4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="1:22" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1">
         <v>38</v>
       </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>60</v>
-      </c>
-      <c r="F4" s="1">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1">
-        <v>1</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="L4" s="1">
-        <v>2</v>
-      </c>
-      <c r="M4" s="1">
-        <v>1</v>
-      </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1">
-        <v>5.3</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>1</v>
-      </c>
-      <c r="R4" s="1">
-        <v>0</v>
-      </c>
-      <c r="S4" s="1">
-        <v>1.25</v>
-      </c>
-      <c r="T4" s="1">
-        <v>1</v>
-      </c>
-      <c r="U4" s="1">
-        <v>65</v>
-      </c>
-      <c r="V4" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="1">
-        <v>34</v>
-      </c>
       <c r="D5" s="1">
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F5" s="1">
         <v>10</v>
@@ -1992,10 +1950,10 @@
         <v>1</v>
       </c>
       <c r="J5" s="1">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="K5" s="1">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="L5" s="1">
         <v>2</v>
@@ -2022,19 +1980,19 @@
         <v>1.25</v>
       </c>
       <c r="T5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U5" s="1">
-        <v>200</v>
+        <v>125</v>
       </c>
       <c r="V5" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -2054,21 +2012,21 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:22" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="C7" s="1">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1">
         <v>10</v>
@@ -2083,10 +2041,10 @@
         <v>1</v>
       </c>
       <c r="J7" s="1">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K7" s="1">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="L7" s="1">
         <v>2</v>
@@ -2113,53 +2071,98 @@
         <v>1.25</v>
       </c>
       <c r="T7" s="1">
+        <v>1</v>
+      </c>
+      <c r="U7" s="1">
+        <v>70</v>
+      </c>
+      <c r="V7" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1">
+        <v>55</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>65</v>
+      </c>
+      <c r="F8" s="1">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1">
         <v>2</v>
       </c>
-      <c r="U7" s="1">
-        <v>125</v>
-      </c>
-      <c r="V7" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-    </row>
-    <row r="9" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>1</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="T8" s="1">
+        <v>1</v>
+      </c>
+      <c r="U8" s="1">
+        <v>55</v>
+      </c>
+      <c r="V8" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="F9" s="1">
         <v>10</v>
@@ -2177,7 +2180,7 @@
         <v>0.8</v>
       </c>
       <c r="K9" s="1">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="L9" s="1">
         <v>2</v>
@@ -2201,33 +2204,33 @@
         <v>0</v>
       </c>
       <c r="S9" s="1">
-        <v>1.25</v>
+        <v>10</v>
       </c>
       <c r="T9" s="1">
         <v>1</v>
       </c>
       <c r="U9" s="1">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="V9" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>72</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="C10" s="1">
+        <v>50</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
         <v>55</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>65</v>
       </c>
       <c r="F10" s="1">
         <v>10</v>
@@ -2257,7 +2260,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="1">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="P10" s="1">
         <v>0.25</v>
@@ -2275,27 +2278,27 @@
         <v>1</v>
       </c>
       <c r="U10" s="1">
+        <v>67</v>
+      </c>
+      <c r="V10" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="1">
         <v>55</v>
       </c>
-      <c r="V10" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="1">
-        <v>38</v>
-      </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="F11" s="1">
         <v>10</v>
@@ -2313,7 +2316,7 @@
         <v>0.8</v>
       </c>
       <c r="K11" s="1">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="L11" s="1">
         <v>2</v>
@@ -2337,124 +2340,124 @@
         <v>0</v>
       </c>
       <c r="S11" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="T11" s="1">
+        <v>2</v>
+      </c>
+      <c r="U11" s="1">
+        <v>100</v>
+      </c>
+      <c r="V11" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+    </row>
+    <row r="13" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>85</v>
+      </c>
+      <c r="F13" s="1">
         <v>10</v>
       </c>
-      <c r="T11" s="1">
-        <v>1</v>
-      </c>
-      <c r="U11" s="1">
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="L13" s="1">
+        <v>2</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>1</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0</v>
+      </c>
+      <c r="S13" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="T13" s="1">
+        <v>1</v>
+      </c>
+      <c r="U13" s="1">
+        <v>58</v>
+      </c>
+      <c r="V13" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="1">
         <v>50</v>
       </c>
-      <c r="V11" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="1">
-        <v>55</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>75</v>
-      </c>
-      <c r="F12" s="1">
-        <v>10</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
-      <c r="I12" s="1">
-        <v>1</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="K12" s="1">
-        <v>1</v>
-      </c>
-      <c r="L12" s="1">
-        <v>2</v>
-      </c>
-      <c r="M12" s="1">
-        <v>1</v>
-      </c>
-      <c r="N12" s="1">
-        <v>0</v>
-      </c>
-      <c r="O12" s="1">
-        <v>3.8</v>
-      </c>
-      <c r="P12" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="Q12" s="1">
-        <v>1</v>
-      </c>
-      <c r="R12" s="1">
-        <v>0</v>
-      </c>
-      <c r="S12" s="1">
-        <v>1.25</v>
-      </c>
-      <c r="T12" s="1">
-        <v>2</v>
-      </c>
-      <c r="U12" s="1">
-        <v>100</v>
-      </c>
-      <c r="V12" s="1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-    </row>
-    <row r="14" spans="1:22" ht="72" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="1">
-        <v>38</v>
-      </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F14" s="1">
         <v>10</v>
@@ -2472,7 +2475,7 @@
         <v>0.8</v>
       </c>
       <c r="K14" s="1">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="L14" s="1">
         <v>2</v>
@@ -2484,7 +2487,7 @@
         <v>0</v>
       </c>
       <c r="O14" s="1">
-        <v>5.3</v>
+        <v>3.8</v>
       </c>
       <c r="P14" s="1">
         <v>0.25</v>
@@ -2502,10 +2505,10 @@
         <v>1</v>
       </c>
       <c r="U14" s="1">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="V14" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="232.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2576,21 +2579,21 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>81</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C16" s="1">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="F16" s="1">
         <v>10</v>
@@ -2605,10 +2608,10 @@
         <v>1</v>
       </c>
       <c r="J16" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="K16" s="1">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="L16" s="1">
         <v>2</v>
@@ -2620,7 +2623,7 @@
         <v>0</v>
       </c>
       <c r="O16" s="1">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P16" s="1">
         <v>0.25</v>
@@ -2632,101 +2635,39 @@
         <v>0</v>
       </c>
       <c r="S16" s="1">
-        <v>10</v>
+        <v>1.25</v>
       </c>
       <c r="T16" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U16" s="1">
-        <v>60</v>
+        <v>350</v>
       </c>
       <c r="V16" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="1">
-        <v>50</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1">
-        <v>60</v>
-      </c>
-      <c r="F17" s="1">
-        <v>10</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1">
-        <v>1</v>
-      </c>
-      <c r="I17" s="1">
-        <v>1</v>
-      </c>
-      <c r="J17" s="1">
-        <v>0.85</v>
-      </c>
-      <c r="K17" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="L17" s="1">
-        <v>2</v>
-      </c>
-      <c r="M17" s="1">
-        <v>1</v>
-      </c>
-      <c r="N17" s="1">
-        <v>0</v>
-      </c>
-      <c r="O17" s="1">
-        <v>3.8</v>
-      </c>
-      <c r="P17" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>1</v>
-      </c>
-      <c r="R17" s="1">
-        <v>0</v>
-      </c>
-      <c r="S17" s="1">
-        <v>1.25</v>
-      </c>
-      <c r="T17" s="1">
-        <v>1</v>
-      </c>
-      <c r="U17" s="1">
-        <v>62</v>
-      </c>
-      <c r="V17" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F18" s="1">
         <v>10</v>
@@ -2744,7 +2685,7 @@
         <v>0.8</v>
       </c>
       <c r="K18" s="1">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="L18" s="1">
         <v>2</v>
@@ -2756,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="O18" s="1">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P18" s="1">
         <v>0.25</v>
@@ -2768,24 +2709,24 @@
         <v>0</v>
       </c>
       <c r="S18" s="1">
-        <v>1.25</v>
+        <v>10</v>
       </c>
       <c r="T18" s="1">
         <v>1</v>
       </c>
       <c r="U18" s="1">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="V18" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1">
         <v>50</v>
@@ -2794,7 +2735,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F19" s="1">
         <v>10</v>
@@ -2812,7 +2753,7 @@
         <v>0.85</v>
       </c>
       <c r="K19" s="1">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="L19" s="1">
         <v>2</v>
@@ -2839,24 +2780,24 @@
         <v>1.25</v>
       </c>
       <c r="T19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U19" s="1">
-        <v>115</v>
+        <v>62</v>
       </c>
       <c r="V19" s="1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C20" s="1">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
@@ -2877,10 +2818,10 @@
         <v>1</v>
       </c>
       <c r="J20" s="1">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="K20" s="1">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="L20" s="1">
         <v>2</v>
@@ -2892,7 +2833,7 @@
         <v>0</v>
       </c>
       <c r="O20" s="1">
-        <v>5.3</v>
+        <v>3.8</v>
       </c>
       <c r="P20" s="1">
         <v>0.25</v>
@@ -2910,18 +2851,18 @@
         <v>1</v>
       </c>
       <c r="U20" s="1">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="V20" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>76</v>
+        <v>21</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="C21" s="1">
         <v>38</v>
@@ -2930,7 +2871,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="F21" s="1">
         <v>10</v>
@@ -2945,7 +2886,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="1">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="K21" s="1">
         <v>0.75</v>
@@ -2960,7 +2901,7 @@
         <v>0</v>
       </c>
       <c r="O21" s="1">
-        <v>3.8</v>
+        <v>5.3</v>
       </c>
       <c r="P21" s="1">
         <v>0.25</v>
@@ -2972,23 +2913,25 @@
         <v>0</v>
       </c>
       <c r="S21" s="1">
-        <v>10</v>
+        <v>1.25</v>
       </c>
       <c r="T21" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U21" s="1">
-        <v>215</v>
+        <v>65</v>
       </c>
       <c r="V21" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="C22" s="1">
         <v>50</v>
       </c>
@@ -2996,7 +2939,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F22" s="1">
         <v>10</v>
@@ -3011,10 +2954,10 @@
         <v>1</v>
       </c>
       <c r="J22" s="1">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="K22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="1">
         <v>2</v>
@@ -3040,20 +2983,31 @@
       <c r="S22" s="1">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="T22" s="1">
+        <v>2</v>
+      </c>
+      <c r="U22" s="1">
+        <v>115</v>
+      </c>
+      <c r="V22" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="C23" s="1">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
       </c>
       <c r="E23" s="1">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="F23" s="1">
         <v>10</v>
@@ -3071,7 +3025,7 @@
         <v>1</v>
       </c>
       <c r="K23" s="1">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="L23" s="1">
         <v>2</v>
@@ -3083,7 +3037,7 @@
         <v>0</v>
       </c>
       <c r="O23" s="1">
-        <v>3.8</v>
+        <v>5.3</v>
       </c>
       <c r="P23" s="1">
         <v>0.25</v>
@@ -3095,24 +3049,33 @@
         <v>0</v>
       </c>
       <c r="S23" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+        <v>1.25</v>
+      </c>
+      <c r="T23" s="1">
+        <v>1</v>
+      </c>
+      <c r="U23" s="1">
+        <v>54</v>
+      </c>
+      <c r="V23" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>48</v>
+        <v>0</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="C24" s="1">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="F24" s="1">
         <v>10</v>
@@ -3127,10 +3090,10 @@
         <v>1</v>
       </c>
       <c r="J24" s="1">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="K24" s="1">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="L24" s="1">
         <v>2</v>
@@ -3154,25 +3117,23 @@
         <v>0</v>
       </c>
       <c r="S24" s="1">
-        <v>1.25</v>
+        <v>10</v>
       </c>
       <c r="T24" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U24" s="1">
-        <v>64</v>
+        <v>215</v>
       </c>
       <c r="V24" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>80</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B25" s="3"/>
       <c r="C25" s="1">
         <v>50</v>
       </c>
@@ -3180,7 +3141,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="F25" s="1">
         <v>10</v>
@@ -3195,10 +3156,10 @@
         <v>1</v>
       </c>
       <c r="J25" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="K25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" s="1">
         <v>2</v>
@@ -3210,7 +3171,7 @@
         <v>0</v>
       </c>
       <c r="O25" s="1">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="P25" s="1">
         <v>0.25</v>
@@ -3224,31 +3185,20 @@
       <c r="S25" s="1">
         <v>1.25</v>
       </c>
-      <c r="T25" s="1">
-        <v>1</v>
-      </c>
-      <c r="U25" s="1">
-        <v>67</v>
-      </c>
-      <c r="V25" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>82</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B26" s="4"/>
       <c r="C26" s="1">
+        <v>20</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
         <v>100</v>
-      </c>
-      <c r="D26" s="1">
-        <v>0</v>
-      </c>
-      <c r="E26" s="1">
-        <v>50</v>
       </c>
       <c r="F26" s="1">
         <v>10</v>
@@ -3266,7 +3216,7 @@
         <v>1</v>
       </c>
       <c r="K26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L26" s="1">
         <v>2</v>
@@ -3290,22 +3240,75 @@
         <v>0</v>
       </c>
       <c r="S26" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="1">
+        <v>45</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>80</v>
+      </c>
+      <c r="F27" s="1">
+        <v>10</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
+      <c r="L27" s="1">
+        <v>2</v>
+      </c>
+      <c r="M27" s="1">
+        <v>1</v>
+      </c>
+      <c r="N27" s="1">
+        <v>0</v>
+      </c>
+      <c r="O27" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="P27" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>1</v>
+      </c>
+      <c r="R27" s="1">
+        <v>0</v>
+      </c>
+      <c r="S27" s="1">
         <v>1.25</v>
       </c>
-      <c r="T26" s="1">
-        <v>4</v>
-      </c>
-      <c r="U26" s="1">
-        <v>350</v>
-      </c>
-      <c r="V26" s="1">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" ht="91.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1" t="s">
-        <v>83</v>
+      <c r="T27" s="1">
+        <v>1</v>
+      </c>
+      <c r="U27" s="1">
+        <v>64</v>
+      </c>
+      <c r="V27" s="1">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -3653,10 +3656,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF4F598-B7D1-4751-B491-BD0874E7F79E}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3667,7 +3670,7 @@
     <col min="5" max="5" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>84</v>
       </c>
@@ -3680,8 +3683,11 @@
       <c r="E1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -3699,7 +3705,7 @@
         <v>Unique</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
@@ -3717,7 +3723,7 @@
         <v>Unique</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
@@ -3735,7 +3741,7 @@
         <v>Unique</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
@@ -3753,7 +3759,7 @@
         <v>Unique</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
@@ -3771,7 +3777,7 @@
         <v>Unique</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
@@ -3789,7 +3795,7 @@
         <v>Unique</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
@@ -3807,7 +3813,7 @@
         <v>Unique</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
@@ -3825,7 +3831,7 @@
         <v>Unique</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="e" vm="9">
         <v>#VALUE!</v>
       </c>
@@ -3840,7 +3846,7 @@
         <v>Unique</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="e" vm="10">
         <v>#VALUE!</v>
       </c>
@@ -3855,7 +3861,7 @@
         <v>Unique</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
@@ -3873,7 +3879,7 @@
         <v>Unique</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="e" vm="12">
         <v>#VALUE!</v>
       </c>
@@ -3891,7 +3897,7 @@
         <v>Unique</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
@@ -3909,7 +3915,7 @@
         <v>Unique</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
@@ -3927,7 +3933,7 @@
         <v>Unique</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="e" vm="15">
         <v>#VALUE!</v>
       </c>

</xml_diff>

<commit_message>
Randomize Items + Upgrades for enemies per floor
</commit_message>
<xml_diff>
--- a/Assets/Numbers.xlsx
+++ b/Assets/Numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\unity\Project\LastDevotion\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99A1D89-BB44-4F34-941F-1A98904242A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C139C8-7463-4663-9330-DE998CC46645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-648" yWindow="1068" windowWidth="17280" windowHeight="10884" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAMPION" sheetId="1" r:id="rId1"/>
@@ -1716,7 +1716,7 @@
   <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="R4" sqref="R4"/>
@@ -3455,7 +3455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{117DB8B5-5D2C-4497-B733-052439D374C4}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -3658,7 +3658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF4F598-B7D1-4751-B491-BD0874E7F79E}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>